<commit_message>
day of the dead
</commit_message>
<xml_diff>
--- a/tabel/delanalyse2.xlsx
+++ b/tabel/delanalyse2.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17329"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17426"/>
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -12,7 +12,7 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14160"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="delanalyse2_indkomstfordeling" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>n</t>
   </si>
@@ -54,6 +54,12 @@
   </si>
   <si>
     <t>Median</t>
+  </si>
+  <si>
+    <t>99. percentil</t>
+  </si>
+  <si>
+    <t>1. percentil</t>
   </si>
 </sst>
 </file>
@@ -62,7 +68,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="44" formatCode="_ &quot;kr.&quot;\ * #,##0.00_ ;_ &quot;kr.&quot;\ * \-#,##0.00_ ;_ &quot;kr.&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="171" formatCode="_-* #,##0\ [$kr.-406]_-;\-* #,##0\ [$kr.-406]_-;_-* &quot;-&quot;??\ [$kr.-406]_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0\ [$kr.-406]_-;\-* #,##0\ [$kr.-406]_-;_-* &quot;-&quot;??\ [$kr.-406]_-;_-@_-"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -146,7 +152,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -163,12 +169,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -484,10 +492,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:K21"/>
+  <dimension ref="A2:K23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -501,7 +509,7 @@
         <v>5</v>
       </c>
       <c r="B2" s="8">
-        <v>221.8</v>
+        <v>226.6</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -509,7 +517,7 @@
         <v>6</v>
       </c>
       <c r="B3" s="9">
-        <v>75.73</v>
+        <v>82.18</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -517,7 +525,7 @@
         <v>7</v>
       </c>
       <c r="B4" s="8">
-        <v>18</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -525,88 +533,108 @@
         <v>8</v>
       </c>
       <c r="B5" s="9">
-        <v>2154.61</v>
+        <v>4492.3419999999996</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="8">
+        <v>130.36439999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="8">
-        <v>154.80000000000001</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="7" t="s">
-        <v>2</v>
-      </c>
       <c r="B7" s="10">
-        <v>176.5</v>
+        <v>156.9204</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="B8" s="10">
-        <v>206.6</v>
+        <v>178.22</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="10">
+        <v>208.35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B9" s="10">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
+      <c r="B10" s="10">
+        <v>249.81</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="B10" s="11">
-        <v>302.10000000000002</v>
-      </c>
-      <c r="K10" s="2"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="12" t="s">
+      <c r="B11" s="10">
+        <v>314.26600000000002</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="11">
+        <v>524.78</v>
+      </c>
+      <c r="K12" s="2"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B11" s="13">
-        <v>205798</v>
-      </c>
-      <c r="K11" s="2"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="K12" s="2"/>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B13" s="13">
+        <v>382131</v>
+      </c>
       <c r="K13" s="2"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="K14" s="2"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="K15" s="1"/>
+      <c r="K15" s="2"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D16" s="14"/>
       <c r="K16" s="2"/>
     </row>
-    <row r="17" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K17" s="3"/>
-    </row>
-    <row r="18" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K18" s="4"/>
-    </row>
-    <row r="19" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K19" s="2"/>
-    </row>
-    <row r="20" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="7:11" x14ac:dyDescent="0.25">
+      <c r="K17" s="1"/>
+    </row>
+    <row r="18" spans="7:11" x14ac:dyDescent="0.25">
+      <c r="K18" s="2"/>
+    </row>
+    <row r="19" spans="7:11" x14ac:dyDescent="0.25">
+      <c r="K19" s="3"/>
+    </row>
+    <row r="20" spans="7:11" x14ac:dyDescent="0.25">
+      <c r="G20" s="14"/>
       <c r="K20" s="4"/>
     </row>
-    <row r="21" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="7:11" x14ac:dyDescent="0.25">
       <c r="K21" s="2"/>
+    </row>
+    <row r="22" spans="7:11" x14ac:dyDescent="0.25">
+      <c r="G22" s="14"/>
+      <c r="K22" s="4"/>
+    </row>
+    <row r="23" spans="7:11" x14ac:dyDescent="0.25">
+      <c r="G23" s="14"/>
+      <c r="K23" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>